<commit_message>
Updated server discovery welcome message
</commit_message>
<xml_diff>
--- a/birthdays.xlsx
+++ b/birthdays.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1127,6 +1127,72 @@
         </is>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>398898064313548820</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Leboge#3392</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>338028125269000199</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Reptile#9182</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>552891291357282304</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Cyber#5379</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Level system bug fix
</commit_message>
<xml_diff>
--- a/birthdays.xlsx
+++ b/birthdays.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1193,6 +1193,28 @@
         </is>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>421837462047031297</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Dkal#4012</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>